<commit_message>
Added interaction functionalities, updated coin rendering on board, updated board design
</commit_message>
<xml_diff>
--- a/docs/Layout.xlsx
+++ b/docs/Layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\Desktop\Python\Programs\pygame_connectfour\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21976CB-AB7A-478A-A6E3-4EF8BD875F95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ED35D7-0229-4611-AD20-01ECBE6E21A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="B1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added intro screen with buttons to set mode
</commit_message>
<xml_diff>
--- a/docs/Layout.xlsx
+++ b/docs/Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\Desktop\Python\Programs\pygame_connectfour\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ED35D7-0229-4611-AD20-01ECBE6E21A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91722117-5320-4160-A27B-C073436DBB2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8835" yWindow="2700" windowWidth="27000" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>INTRO SCREEN</t>
+  </si>
+  <si>
+    <t>GAME SCREEN</t>
+  </si>
+  <si>
+    <t>CONNECT FOUR!</t>
+  </si>
+  <si>
+    <t>PLAY VS COMPUTER</t>
+  </si>
+  <si>
+    <t>PLAY VS PLAYER 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and [DOWN] arrow key to confirm.</t>
+  </si>
+  <si>
+    <t>Use [LEFT] and [RIGHT] arrow keys to navigate through the columns</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,8 +60,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Prequel Demo Shadow Italic"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Prequel Demo Shadow Italic"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="40"/>
+      <color theme="1"/>
+      <name val="Prequel Demo Shadow Italic"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -54,6 +104,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -162,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -181,6 +243,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M11"/>
+  <dimension ref="B1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,189 +557,395 @@
     <col min="2" max="13" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="2:13" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="7">
-        <v>64</v>
-      </c>
-      <c r="D2" s="7">
-        <v>64</v>
-      </c>
-      <c r="E2" s="7">
-        <v>64</v>
-      </c>
-      <c r="F2" s="7">
-        <v>64</v>
-      </c>
-      <c r="G2" s="7">
-        <v>64</v>
-      </c>
-      <c r="H2" s="7">
-        <v>64</v>
-      </c>
-      <c r="I2" s="7">
-        <v>64</v>
-      </c>
-      <c r="J2" s="7">
-        <v>64</v>
-      </c>
-      <c r="K2" s="7">
-        <v>64</v>
-      </c>
-      <c r="L2" s="7">
-        <v>64</v>
-      </c>
-      <c r="M2" s="7">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8">
-        <v>64</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="P2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+    </row>
+    <row r="3" spans="2:26" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="7">
+        <v>64</v>
+      </c>
+      <c r="D3" s="7">
+        <v>64</v>
+      </c>
+      <c r="E3" s="7">
+        <v>64</v>
+      </c>
+      <c r="F3" s="7">
+        <v>64</v>
+      </c>
+      <c r="G3" s="7">
+        <v>64</v>
+      </c>
+      <c r="H3" s="7">
+        <v>64</v>
+      </c>
+      <c r="I3" s="7">
+        <v>64</v>
+      </c>
+      <c r="J3" s="7">
+        <v>64</v>
+      </c>
+      <c r="K3" s="7">
+        <v>64</v>
+      </c>
+      <c r="L3" s="7">
+        <v>64</v>
+      </c>
+      <c r="M3" s="7">
+        <v>64</v>
+      </c>
+      <c r="P3" s="7">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>64</v>
+      </c>
+      <c r="R3" s="7">
+        <v>64</v>
+      </c>
+      <c r="S3" s="7">
+        <v>64</v>
+      </c>
+      <c r="T3" s="7">
+        <v>64</v>
+      </c>
+      <c r="U3" s="7">
+        <v>64</v>
+      </c>
+      <c r="V3" s="7">
+        <v>64</v>
+      </c>
+      <c r="W3" s="7">
+        <v>64</v>
+      </c>
+      <c r="X3" s="7">
+        <v>64</v>
+      </c>
+      <c r="Y3" s="7">
+        <v>64</v>
+      </c>
+      <c r="Z3" s="7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8">
         <v>64</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+      <c r="O4" s="8">
+        <v>64</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="3"/>
+    </row>
+    <row r="5" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
         <v>64</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="18"/>
+      <c r="D5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="19"/>
+      <c r="O5" s="8">
+        <v>64</v>
+      </c>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8">
         <v>64</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="18"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="19"/>
+      <c r="O6" s="8">
+        <v>64</v>
+      </c>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <v>64</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
+      <c r="E7" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="19"/>
+      <c r="O7" s="8">
+        <v>64</v>
+      </c>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8">
         <v>64</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="E8" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="19"/>
+      <c r="O8" s="8">
+        <v>64</v>
+      </c>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8">
         <v>64</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="2:13" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="18"/>
+      <c r="D9" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="19"/>
+      <c r="O9" s="8">
+        <v>64</v>
+      </c>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="6"/>
+    </row>
+    <row r="10" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8">
         <v>64</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="2:13" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="18"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="19"/>
+      <c r="O10" s="8">
+        <v>64</v>
+      </c>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8">
         <v>64</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="19"/>
+      <c r="O11" s="8">
+        <v>64</v>
+      </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="6"/>
+    </row>
+    <row r="12" spans="2:26" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="8">
+        <v>64</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="22"/>
+      <c r="O12" s="8">
+        <v>64</v>
+      </c>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="E8:K8"/>
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="P2:Z2"/>
+    <mergeCell ref="D9:G10"/>
+    <mergeCell ref="I9:L10"/>
+    <mergeCell ref="D5:L6"/>
+    <mergeCell ref="E7:K7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added check for winner functionality and winner screen
</commit_message>
<xml_diff>
--- a/docs/Layout.xlsx
+++ b/docs/Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\Desktop\Python\Programs\pygame_connectfour\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91722117-5320-4160-A27B-C073436DBB2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B23D7-230F-4B12-B2DC-A12B3FF7FCE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8835" yWindow="2700" windowWidth="27000" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>INTRO SCREEN</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Use [LEFT] and [RIGHT] arrow keys to navigate through the columns</t>
+  </si>
+  <si>
+    <t>WINNING SCREEN</t>
+  </si>
+  <si>
+    <t>f"PLAYER {player} WON!"</t>
   </si>
 </sst>
 </file>
@@ -224,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -252,20 +258,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Z12"/>
+  <dimension ref="B1:AM12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5:AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,38 +569,51 @@
     <col min="2" max="13" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="23" t="s">
+    <row r="2" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="P2" s="23" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="P2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AC2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
     </row>
-    <row r="3" spans="2:26" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:39" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="7">
         <v>64</v>
       </c>
@@ -655,8 +680,41 @@
       <c r="Z3" s="7">
         <v>64</v>
       </c>
+      <c r="AC3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AD3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AE3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AF3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AG3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AH3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AI3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AJ3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AK3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AL3" s="7">
+        <v>64</v>
+      </c>
+      <c r="AM3" s="7">
+        <v>64</v>
+      </c>
     </row>
-    <row r="4" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8">
         <v>64</v>
       </c>
@@ -685,23 +743,37 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="3"/>
+      <c r="AB4" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="16"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="17"/>
     </row>
-    <row r="5" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
         <v>64</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
       <c r="M5" s="19"/>
       <c r="O5" s="8">
         <v>64</v>
@@ -717,21 +789,35 @@
       <c r="X5" s="13"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="6"/>
+      <c r="AB5" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="14"/>
+      <c r="AL5" s="14"/>
+      <c r="AM5" s="19"/>
     </row>
-    <row r="6" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8">
         <v>64</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
       <c r="M6" s="19"/>
       <c r="O6" s="8">
         <v>64</v>
@@ -747,22 +833,35 @@
       <c r="X6" s="9"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="6"/>
+      <c r="AB6" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="14"/>
+      <c r="AF6" s="30"/>
+      <c r="AG6" s="30"/>
+      <c r="AH6" s="30"/>
+      <c r="AI6" s="30"/>
+      <c r="AJ6" s="30"/>
+      <c r="AK6" s="30"/>
+      <c r="AL6" s="14"/>
+      <c r="AM6" s="19"/>
     </row>
-    <row r="7" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <v>64</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
       <c r="L7" s="5"/>
       <c r="M7" s="19"/>
       <c r="O7" s="8">
@@ -779,22 +878,38 @@
       <c r="X7" s="9"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="6"/>
+      <c r="AB7" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="30"/>
+      <c r="AF7" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29"/>
+      <c r="AI7" s="29"/>
+      <c r="AJ7" s="29"/>
+      <c r="AK7" s="30"/>
+      <c r="AL7" s="14"/>
+      <c r="AM7" s="19"/>
     </row>
-    <row r="8" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8">
         <v>64</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="5"/>
       <c r="M8" s="19"/>
       <c r="O8" s="8">
@@ -811,25 +926,39 @@
       <c r="X8" s="9"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="6"/>
+      <c r="AB8" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="30"/>
+      <c r="AF8" s="29"/>
+      <c r="AG8" s="29"/>
+      <c r="AH8" s="29"/>
+      <c r="AI8" s="29"/>
+      <c r="AJ8" s="29"/>
+      <c r="AK8" s="30"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="19"/>
     </row>
-    <row r="9" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8">
         <v>64</v>
       </c>
       <c r="C9" s="18"/>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
       <c r="M9" s="19"/>
       <c r="O9" s="8">
         <v>64</v>
@@ -845,21 +974,35 @@
       <c r="X9" s="9"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="6"/>
+      <c r="AB9" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="30"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
+      <c r="AH9" s="29"/>
+      <c r="AI9" s="29"/>
+      <c r="AJ9" s="29"/>
+      <c r="AK9" s="30"/>
+      <c r="AL9" s="14"/>
+      <c r="AM9" s="19"/>
     </row>
-    <row r="10" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8">
         <v>64</v>
       </c>
       <c r="C10" s="18"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
       <c r="M10" s="19"/>
       <c r="O10" s="8">
         <v>64</v>
@@ -875,8 +1018,22 @@
       <c r="X10" s="9"/>
       <c r="Y10" s="5"/>
       <c r="Z10" s="6"/>
+      <c r="AB10" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="14"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="30"/>
+      <c r="AI10" s="30"/>
+      <c r="AJ10" s="30"/>
+      <c r="AK10" s="30"/>
+      <c r="AL10" s="14"/>
+      <c r="AM10" s="19"/>
     </row>
-    <row r="11" spans="2:26" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:39" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8">
         <v>64</v>
       </c>
@@ -884,7 +1041,7 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="25"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -905,15 +1062,29 @@
       <c r="X11" s="9"/>
       <c r="Y11" s="5"/>
       <c r="Z11" s="6"/>
+      <c r="AB11" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="14"/>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14"/>
+      <c r="AG11" s="14"/>
+      <c r="AH11" s="14"/>
+      <c r="AI11" s="14"/>
+      <c r="AJ11" s="14"/>
+      <c r="AK11" s="14"/>
+      <c r="AL11" s="14"/>
+      <c r="AM11" s="19"/>
     </row>
-    <row r="12" spans="2:26" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:39" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="8">
         <v>64</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="28"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
@@ -935,9 +1106,25 @@
       <c r="X12" s="11"/>
       <c r="Y12" s="11"/>
       <c r="Z12" s="12"/>
+      <c r="AB12" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="21"/>
+      <c r="AE12" s="21"/>
+      <c r="AF12" s="21"/>
+      <c r="AG12" s="21"/>
+      <c r="AH12" s="21"/>
+      <c r="AI12" s="21"/>
+      <c r="AJ12" s="21"/>
+      <c r="AK12" s="21"/>
+      <c r="AL12" s="21"/>
+      <c r="AM12" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="AC2:AM2"/>
+    <mergeCell ref="AF7:AJ9"/>
     <mergeCell ref="E8:K8"/>
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="P2:Z2"/>

</xml_diff>

<commit_message>
Added reset functionality, solved winner label bug
</commit_message>
<xml_diff>
--- a/docs/Layout.xlsx
+++ b/docs/Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\Desktop\Python\Programs\pygame_connectfour\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B23D7-230F-4B12-B2DC-A12B3FF7FCE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F4C5DA-8B73-4234-82D2-B731BEF8B79D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18315" yWindow="4380" windowWidth="21600" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>INTRO SCREEN</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>f"PLAYER {player} WON!"</t>
+  </si>
+  <si>
+    <t>RESTART</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +125,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -230,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -260,11 +269,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -272,11 +284,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AM12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5:AJ5"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AI4" sqref="AC4:AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,17 +775,17 @@
         <v>64</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
       <c r="M5" s="19"/>
       <c r="O5" s="8">
         <v>64</v>
@@ -794,13 +806,17 @@
       </c>
       <c r="AC5" s="18"/>
       <c r="AD5" s="14"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
+      <c r="AE5" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="30"/>
+      <c r="AI5" s="30"/>
+      <c r="AJ5" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK5" s="31"/>
       <c r="AL5" s="14"/>
       <c r="AM5" s="19"/>
     </row>
@@ -809,15 +825,15 @@
         <v>64</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
       <c r="M6" s="19"/>
       <c r="O6" s="8">
         <v>64</v>
@@ -838,12 +854,12 @@
       </c>
       <c r="AC6" s="18"/>
       <c r="AD6" s="14"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
-      <c r="AH6" s="30"/>
-      <c r="AI6" s="30"/>
-      <c r="AJ6" s="30"/>
-      <c r="AK6" s="30"/>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="25"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="25"/>
+      <c r="AJ6" s="25"/>
+      <c r="AK6" s="25"/>
       <c r="AL6" s="14"/>
       <c r="AM6" s="19"/>
     </row>
@@ -853,15 +869,15 @@
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="5"/>
       <c r="M7" s="19"/>
       <c r="O7" s="8">
@@ -883,15 +899,12 @@
       </c>
       <c r="AC7" s="18"/>
       <c r="AD7" s="14"/>
-      <c r="AE7" s="30"/>
-      <c r="AF7" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG7" s="29"/>
-      <c r="AH7" s="29"/>
-      <c r="AI7" s="29"/>
-      <c r="AJ7" s="29"/>
-      <c r="AK7" s="30"/>
+      <c r="AE7" s="25"/>
+      <c r="AG7" s="25"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="25"/>
+      <c r="AJ7" s="25"/>
+      <c r="AK7" s="25"/>
       <c r="AL7" s="14"/>
       <c r="AM7" s="19"/>
     </row>
@@ -901,15 +914,15 @@
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
       <c r="L8" s="5"/>
       <c r="M8" s="19"/>
       <c r="O8" s="8">
@@ -931,13 +944,13 @@
       </c>
       <c r="AC8" s="18"/>
       <c r="AD8" s="14"/>
-      <c r="AE8" s="30"/>
-      <c r="AF8" s="29"/>
-      <c r="AG8" s="29"/>
-      <c r="AH8" s="29"/>
-      <c r="AI8" s="29"/>
-      <c r="AJ8" s="29"/>
-      <c r="AK8" s="30"/>
+      <c r="AE8" s="25"/>
+      <c r="AF8" s="25"/>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="25"/>
+      <c r="AJ8" s="25"/>
+      <c r="AK8" s="25"/>
       <c r="AL8" s="14"/>
       <c r="AM8" s="19"/>
     </row>
@@ -946,19 +959,19 @@
         <v>64</v>
       </c>
       <c r="C9" s="18"/>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
       <c r="M9" s="19"/>
       <c r="O9" s="8">
         <v>64</v>
@@ -979,13 +992,13 @@
       </c>
       <c r="AC9" s="18"/>
       <c r="AD9" s="14"/>
-      <c r="AE9" s="30"/>
-      <c r="AF9" s="29"/>
-      <c r="AG9" s="29"/>
-      <c r="AH9" s="29"/>
-      <c r="AI9" s="29"/>
-      <c r="AJ9" s="29"/>
-      <c r="AK9" s="30"/>
+      <c r="AE9" s="25"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="25"/>
+      <c r="AJ9" s="25"/>
+      <c r="AK9" s="25"/>
       <c r="AL9" s="14"/>
       <c r="AM9" s="19"/>
     </row>
@@ -994,15 +1007,15 @@
         <v>64</v>
       </c>
       <c r="C10" s="18"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
       <c r="M10" s="19"/>
       <c r="O10" s="8">
         <v>64</v>
@@ -1023,13 +1036,13 @@
       </c>
       <c r="AC10" s="18"/>
       <c r="AD10" s="14"/>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="30"/>
-      <c r="AG10" s="30"/>
-      <c r="AH10" s="30"/>
-      <c r="AI10" s="30"/>
-      <c r="AJ10" s="30"/>
-      <c r="AK10" s="30"/>
+      <c r="AE10" s="25"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="25"/>
+      <c r="AI10" s="25"/>
+      <c r="AJ10" s="25"/>
+      <c r="AK10" s="25"/>
       <c r="AL10" s="14"/>
       <c r="AM10" s="19"/>
     </row>
@@ -1122,9 +1135,8 @@
       <c r="AM12" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="AC2:AM2"/>
-    <mergeCell ref="AF7:AJ9"/>
     <mergeCell ref="E8:K8"/>
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="P2:Z2"/>
@@ -1132,6 +1144,8 @@
     <mergeCell ref="I9:L10"/>
     <mergeCell ref="D5:L6"/>
     <mergeCell ref="E7:K7"/>
+    <mergeCell ref="AE5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>